<commit_message>
Added installation guide and created script for both pre and post LLM data collection.
</commit_message>
<xml_diff>
--- a/excel_files/Stack Overflow Data Collection.xlsx
+++ b/excel_files/Stack Overflow Data Collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coltonpalfrey/Desktop/PASCL RA/Stack-Overflow-Data-Analysis/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C1D17E-602A-B243-A81F-2DECF0B44675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6211DC8-E7B3-924C-9E72-79FB7E8B9994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{1E05B25D-E817-2248-B7C5-0489F78289AB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="5" xr2:uid="{1E05B25D-E817-2248-B7C5-0489F78289AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Pre LLM monthly data" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="50">
   <si>
     <t>Start Date</t>
   </si>
@@ -189,24 +189,21 @@
   <si>
     <t>Avg length of body per answer</t>
   </si>
+  <si>
+    <t>Avg highest score for a question answered to a question with over 500 views</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -247,15 +244,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C94A1581-E026-5849-94E2-0B317A96ACA8}">
   <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,1204 +608,1273 @@
     <col min="13" max="13" width="20.1640625" customWidth="1"/>
     <col min="14" max="14" width="18.83203125" customWidth="1"/>
     <col min="15" max="15" width="24.6640625" customWidth="1"/>
-    <col min="16" max="16" width="14.33203125" customWidth="1"/>
+    <col min="16" max="16" width="61.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="P1" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>43435</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>43465</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>307828</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <f>ROUND(C2/(B2-A2), 0)</f>
         <v>10261</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>1</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>129945</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <f>(C2-F2)</f>
         <v>177883</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <f>ROUND(G2/(B2-A2), 0)</f>
         <v>5929</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>1887</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="5">
         <v>1</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="2">
         <v>1679</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="2">
         <v>116899</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="2">
         <v>109935</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="5">
         <f>ROUND(M2/(B2-A2), 0)</f>
         <v>3665</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2" s="2">
         <v>939</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="P2" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>43466</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>43496</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>343456</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <f t="shared" ref="D3:D23" si="0">ROUND(C3/(B3-A3), 0)</f>
         <v>11449</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>144063</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <f t="shared" ref="G3:G23" si="1">(C3-F3)</f>
         <v>199393</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <f t="shared" ref="H3:H23" si="2">ROUND(G3/(B3-A3), 0)</f>
         <v>6646</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="5">
         <v>1871</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <v>1</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <v>1700</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="2">
         <v>136207</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="2">
         <v>110641</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="5">
         <f t="shared" ref="N3:N23" si="3">ROUND(M3/(B3-A3), 0)</f>
         <v>3688</v>
       </c>
-      <c r="O3" s="1">
+      <c r="O3" s="2">
         <v>950</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="P3" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>43497</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>43524</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>335057</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <f t="shared" si="0"/>
         <v>12410</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>1</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>140790</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <f t="shared" si="1"/>
         <v>194267</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <f t="shared" si="2"/>
         <v>7195</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>1797</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>1</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>1685</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="2">
         <v>125972</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="2">
         <v>103668</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="5">
         <f t="shared" si="3"/>
         <v>3840</v>
       </c>
-      <c r="O4" s="1">
+      <c r="O4" s="2">
         <v>944</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="P4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>43525</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>43555</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>374700</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <f t="shared" si="0"/>
         <v>12490</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>1</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>158869</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <f t="shared" si="1"/>
         <v>215831</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <f t="shared" si="2"/>
         <v>7194</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>1752</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>1</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <v>1689</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="2">
         <v>143373</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="2">
         <v>122739</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="5">
         <f t="shared" si="3"/>
         <v>4091</v>
       </c>
-      <c r="O5" s="1">
+      <c r="O5" s="2">
         <v>946</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="P5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>43556</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>43585</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>348084</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <f t="shared" si="0"/>
         <v>12003</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>1</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>148561</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <f t="shared" si="1"/>
         <v>199523</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <f t="shared" si="2"/>
         <v>6880</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>1648</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <v>1</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="5">
         <v>1711</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="2">
         <v>138384</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="2">
         <v>125627</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="5">
         <f t="shared" si="3"/>
         <v>4332</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6" s="2">
         <v>939</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="P6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>43586</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>43616</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>342417</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <f t="shared" si="0"/>
         <v>11414</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>1</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>146982</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <f t="shared" si="1"/>
         <v>195435</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <f t="shared" si="2"/>
         <v>6515</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>1519</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <v>1</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="5">
         <v>1718</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="2">
         <v>141902</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="2">
         <v>135440</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="5">
         <f t="shared" si="3"/>
         <v>4515</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O7" s="2">
         <v>951</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="P7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>43617</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>43646</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>313933</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <f t="shared" si="0"/>
         <v>10825</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>1</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>134225</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <f t="shared" si="1"/>
         <v>179708</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <f t="shared" si="2"/>
         <v>6197</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <v>1731</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <v>1</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="5">
         <v>1716</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="2">
         <v>129940</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="2">
         <v>122298</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="5">
         <f t="shared" si="3"/>
         <v>4217</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8" s="2">
         <v>953</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="P8" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>43647</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>43677</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>339572</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <f t="shared" si="0"/>
         <v>11319</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>1</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>145714</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <f t="shared" si="1"/>
         <v>193858</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <f t="shared" si="2"/>
         <v>6462</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>1593</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>1</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <v>1726</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="2">
         <v>135123</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="2">
         <v>121836</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="5">
         <f t="shared" si="3"/>
         <v>4061</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O9" s="2">
         <v>941</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="P9" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>43678</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>43708</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>321592</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <f t="shared" si="0"/>
         <v>10720</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>1</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>135378</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <f t="shared" si="1"/>
         <v>186214</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <f t="shared" si="2"/>
         <v>6207</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <v>1569</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="5">
         <v>1</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="5">
         <v>1740</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="2">
         <v>131642</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="2">
         <v>122614</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="5">
         <f t="shared" si="3"/>
         <v>4087</v>
       </c>
-      <c r="O10" s="1">
+      <c r="O10" s="2">
         <v>946</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="P10" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>43709</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>43738</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>311774</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <f t="shared" si="0"/>
         <v>10751</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>1</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>132258</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <f t="shared" si="1"/>
         <v>179516</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <f t="shared" si="2"/>
         <v>6190</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <v>1597</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="5">
         <v>1</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="5">
         <v>1698</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="2">
         <v>131286</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="2">
         <v>115461</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="5">
         <f t="shared" si="3"/>
         <v>3981</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O11" s="2">
         <v>945</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="P11" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>43739</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>43769</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>345366</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <f t="shared" si="0"/>
         <v>11512</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>1</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>147794</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <f t="shared" si="1"/>
         <v>197572</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <f t="shared" si="2"/>
         <v>6586</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="2">
         <v>1524</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="5">
         <v>1</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="5">
         <v>1689</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L12" s="2">
         <v>149463</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M12" s="2">
         <v>130915</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="5">
         <f t="shared" si="3"/>
         <v>4364</v>
       </c>
-      <c r="O12" s="1">
+      <c r="O12" s="2">
         <v>939</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="P12" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>43770</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>43799</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>343404</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <f t="shared" si="0"/>
         <v>11842</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>1</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>145998</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <f t="shared" si="1"/>
         <v>197406</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <f t="shared" si="2"/>
         <v>6807</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="2">
         <v>1433</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="5">
         <v>1</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="5">
         <v>1708</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="2">
         <v>143197</v>
       </c>
-      <c r="M13" s="1">
+      <c r="M13" s="2">
         <v>131539</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="5">
         <f t="shared" si="3"/>
         <v>4536</v>
       </c>
-      <c r="O13" s="1">
+      <c r="O13" s="2">
         <v>946</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="P13" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>43800</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>43830</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>306925</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <f t="shared" si="0"/>
         <v>10231</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>1</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>129894</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="5">
         <f t="shared" si="1"/>
         <v>177031</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="5">
         <f t="shared" si="2"/>
         <v>5901</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="2">
         <v>1514</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="5">
         <v>1</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="5">
         <v>1754</v>
       </c>
-      <c r="L14" s="1">
+      <c r="L14" s="2">
         <v>152599</v>
       </c>
-      <c r="M14" s="1">
+      <c r="M14" s="2">
         <v>151088</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="5">
         <f t="shared" si="3"/>
         <v>5036</v>
       </c>
-      <c r="O14" s="1">
+      <c r="O14" s="2">
         <v>963</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="P14" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>43831</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>43861</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>333749</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <f t="shared" si="0"/>
         <v>11125</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>1</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <v>142240</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <f t="shared" si="1"/>
         <v>191509</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <f t="shared" si="2"/>
         <v>6384</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="2">
         <v>1519</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="5">
         <v>1</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="5">
         <v>1739</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L15" s="2">
         <v>165206</v>
       </c>
-      <c r="M15" s="1">
+      <c r="M15" s="2">
         <v>152105</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="5">
         <f t="shared" si="3"/>
         <v>5070</v>
       </c>
-      <c r="O15" s="1">
+      <c r="O15" s="2">
         <v>962</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="P15" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>43862</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>43889</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>319135</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <f t="shared" si="0"/>
         <v>11820</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>1</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <v>137391</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="5">
         <f t="shared" si="1"/>
         <v>181744</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="5">
         <f t="shared" si="2"/>
         <v>6731</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="2">
         <v>1460</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J16" s="5">
         <v>1</v>
       </c>
-      <c r="K16" s="6">
+      <c r="K16" s="5">
         <v>1738</v>
       </c>
-      <c r="L16" s="1">
+      <c r="L16" s="2">
         <v>146845</v>
       </c>
-      <c r="M16" s="1">
+      <c r="M16" s="2">
         <v>136569</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="5">
         <f t="shared" si="3"/>
         <v>5058</v>
       </c>
-      <c r="O16" s="1">
+      <c r="O16" s="2">
         <v>961</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="P16" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>43891</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>43921</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>339246</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <f t="shared" si="0"/>
         <v>11308</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>1</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="2">
         <v>150213</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <f t="shared" si="1"/>
         <v>189033</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <f t="shared" si="2"/>
         <v>6301</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="2">
         <v>1343</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J17" s="5">
         <v>1</v>
       </c>
-      <c r="K17" s="6">
+      <c r="K17" s="5">
         <v>1751</v>
       </c>
-      <c r="L17" s="1">
+      <c r="L17" s="2">
         <v>165877</v>
       </c>
-      <c r="M17" s="1">
+      <c r="M17" s="2">
         <v>163194</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="5">
         <f t="shared" si="3"/>
         <v>5440</v>
       </c>
-      <c r="O17" s="1">
+      <c r="O17" s="2">
         <v>965</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="P17" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>43922</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <v>43951</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>400351</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <f t="shared" si="0"/>
         <v>13805</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>1</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="2">
         <v>176917</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="5">
         <f t="shared" si="1"/>
         <v>223434</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="5">
         <f t="shared" si="2"/>
         <v>7705</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="2">
         <v>1308</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J18" s="5">
         <v>1</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="5">
         <v>1733</v>
       </c>
-      <c r="L18" s="1">
+      <c r="L18" s="2">
         <v>252284</v>
       </c>
-      <c r="M18" s="1">
+      <c r="M18" s="2">
         <v>171427</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="5">
         <f t="shared" si="3"/>
         <v>5911</v>
       </c>
-      <c r="O18" s="1">
+      <c r="O18" s="2">
         <v>956</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="P18" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>43952</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>43982</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>419437</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <f t="shared" si="0"/>
         <v>13981</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>1</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <v>183207</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="5">
         <f t="shared" si="1"/>
         <v>236230</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="5">
         <f t="shared" si="2"/>
         <v>7874</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="2">
         <v>1277</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="5">
         <v>1</v>
       </c>
-      <c r="K19" s="6">
+      <c r="K19" s="5">
         <v>1725</v>
       </c>
-      <c r="L19" s="1">
+      <c r="L19" s="2">
         <v>193311</v>
       </c>
-      <c r="M19" s="1">
+      <c r="M19" s="2">
         <v>175555</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="5">
         <f t="shared" si="3"/>
         <v>5852</v>
       </c>
-      <c r="O19" s="1">
+      <c r="O19" s="2">
         <v>957</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="P19" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
         <v>43983</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <v>44012</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>382283</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <f t="shared" si="0"/>
         <v>13182</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>1</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>166528</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="5">
         <f t="shared" si="1"/>
         <v>215755</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="5">
         <f t="shared" si="2"/>
         <v>7440</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="2">
         <v>1291</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J20" s="5">
         <v>1</v>
       </c>
-      <c r="K20" s="6">
+      <c r="K20" s="5">
         <v>1740</v>
       </c>
-      <c r="L20" s="1">
+      <c r="L20" s="2">
         <v>178356</v>
       </c>
-      <c r="M20" s="1">
+      <c r="M20" s="2">
         <v>177517</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="5">
         <f t="shared" si="3"/>
         <v>6121</v>
       </c>
-      <c r="O20" s="1">
+      <c r="O20" s="2">
         <v>960</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="P20" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>44013</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <v>44043</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>373541</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <f t="shared" si="0"/>
         <v>12451</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>1</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <v>161728</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="5">
         <f t="shared" si="1"/>
         <v>211813</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="5">
         <f t="shared" si="2"/>
         <v>7060</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="2">
         <v>1314</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J21" s="5">
         <v>1</v>
       </c>
-      <c r="K21" s="6">
+      <c r="K21" s="5">
         <v>1799</v>
       </c>
-      <c r="L21" s="1">
+      <c r="L21" s="2">
         <v>166996</v>
       </c>
-      <c r="M21" s="1">
+      <c r="M21" s="2">
         <v>165273</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="5">
         <f t="shared" si="3"/>
         <v>5509</v>
       </c>
-      <c r="O21" s="1">
+      <c r="O21" s="2">
         <v>975</v>
       </c>
-    </row>
-    <row r="22" spans="1:23" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="P21" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
         <v>44044</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <v>44074</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>334163</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <f t="shared" si="0"/>
         <v>11139</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>1</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>143950</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="5">
         <f t="shared" si="1"/>
         <v>190213</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="5">
         <f t="shared" si="2"/>
         <v>6340</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="2">
         <v>1292</v>
       </c>
-      <c r="J22" s="6">
+      <c r="J22" s="5">
         <v>1</v>
       </c>
-      <c r="K22" s="6">
+      <c r="K22" s="5">
         <v>1833</v>
       </c>
-      <c r="L22" s="1">
+      <c r="L22" s="2">
         <v>158378</v>
       </c>
-      <c r="M22" s="1">
+      <c r="M22" s="2">
         <v>157018</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="5">
         <f t="shared" si="3"/>
         <v>5234</v>
       </c>
-      <c r="O22" s="1">
+      <c r="O22" s="2">
         <v>988</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="P22" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
         <v>44075</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="6">
         <v>44104</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>316956</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <f t="shared" si="0"/>
         <v>10930</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
         <v>1</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>136988</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="5">
         <f t="shared" si="1"/>
         <v>179968</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="5">
         <f t="shared" si="2"/>
         <v>6206</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="2">
         <v>1261</v>
       </c>
-      <c r="J23" s="6">
+      <c r="J23" s="5">
         <v>0</v>
       </c>
-      <c r="K23" s="6">
+      <c r="K23" s="5">
         <v>1807</v>
       </c>
-      <c r="L23" s="1">
+      <c r="L23" s="2">
         <v>161198</v>
       </c>
-      <c r="M23" s="1">
+      <c r="M23" s="2">
         <v>156566</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="5">
         <f t="shared" si="3"/>
         <v>5399</v>
       </c>
-      <c r="O23" s="1">
+      <c r="O23" s="2">
         <v>990</v>
       </c>
+      <c r="P23" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
-      <c r="W25" s="2"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1831,84 +1896,84 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4">
+      <c r="C1" s="3">
         <v>0</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="3">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="3">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="3">
         <v>0.125</v>
       </c>
-      <c r="G1" s="4">
+      <c r="G1" s="3">
         <v>0.16666666666666666</v>
       </c>
-      <c r="H1" s="4">
+      <c r="H1" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="I1" s="4">
+      <c r="I1" s="3">
         <v>0.25</v>
       </c>
-      <c r="J1" s="4">
+      <c r="J1" s="3">
         <v>0.29166666666666669</v>
       </c>
-      <c r="K1" s="4">
+      <c r="K1" s="3">
         <v>0.33333333333333331</v>
       </c>
-      <c r="L1" s="4">
+      <c r="L1" s="3">
         <v>0.375</v>
       </c>
-      <c r="M1" s="4">
+      <c r="M1" s="3">
         <v>0.41666666666666669</v>
       </c>
-      <c r="N1" s="4">
+      <c r="N1" s="3">
         <v>0.45833333333333331</v>
       </c>
-      <c r="O1" s="4">
+      <c r="O1" s="3">
         <v>0.5</v>
       </c>
-      <c r="P1" s="4">
+      <c r="P1" s="3">
         <v>0.54166666666666663</v>
       </c>
-      <c r="Q1" s="4">
+      <c r="Q1" s="3">
         <v>0.58333333333333337</v>
       </c>
-      <c r="R1" s="4">
+      <c r="R1" s="3">
         <v>0.625</v>
       </c>
-      <c r="S1" s="4">
+      <c r="S1" s="3">
         <v>0.66666666666666663</v>
       </c>
-      <c r="T1" s="4">
+      <c r="T1" s="3">
         <v>0.70833333333333337</v>
       </c>
-      <c r="U1" s="4">
+      <c r="U1" s="3">
         <v>0.75</v>
       </c>
-      <c r="V1" s="4">
+      <c r="V1" s="3">
         <v>0.79166666666666663</v>
       </c>
-      <c r="W1" s="4">
+      <c r="W1" s="3">
         <v>0.83333333333333337</v>
       </c>
-      <c r="X1" s="4">
+      <c r="X1" s="3">
         <v>0.875</v>
       </c>
-      <c r="Y1" s="4">
+      <c r="Y1" s="3">
         <v>0.91666666666666663</v>
       </c>
-      <c r="Z1" s="4">
+      <c r="Z1" s="3">
         <v>0.95833333333333337</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>43435</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>43465</v>
       </c>
       <c r="C2">
@@ -1985,10 +2050,10 @@
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>43466</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>43496</v>
       </c>
       <c r="C3">
@@ -2065,10 +2130,10 @@
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>43497</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>43524</v>
       </c>
       <c r="C4">
@@ -2145,10 +2210,10 @@
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>43525</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>43555</v>
       </c>
       <c r="C5">
@@ -2225,10 +2290,10 @@
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>43556</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>43585</v>
       </c>
       <c r="C6">
@@ -2305,10 +2370,10 @@
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>43586</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>43616</v>
       </c>
       <c r="C7">
@@ -2385,10 +2450,10 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>43617</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>43646</v>
       </c>
       <c r="C8">
@@ -2465,10 +2530,10 @@
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>43647</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>43677</v>
       </c>
       <c r="C9">
@@ -2545,10 +2610,10 @@
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>43678</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>43708</v>
       </c>
       <c r="C10">
@@ -2625,10 +2690,10 @@
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>43709</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>43738</v>
       </c>
       <c r="C11">
@@ -2705,10 +2770,10 @@
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>43739</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>43769</v>
       </c>
       <c r="C12">
@@ -2785,10 +2850,10 @@
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>43770</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>43799</v>
       </c>
       <c r="C13">
@@ -2865,10 +2930,10 @@
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>43800</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>43830</v>
       </c>
       <c r="C14">
@@ -2945,10 +3010,10 @@
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>43831</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>43861</v>
       </c>
       <c r="C15">
@@ -3025,10 +3090,10 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>43862</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>43889</v>
       </c>
       <c r="C16">
@@ -3105,10 +3170,10 @@
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>43891</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>43921</v>
       </c>
       <c r="C17">
@@ -3185,10 +3250,10 @@
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>43922</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>43951</v>
       </c>
       <c r="C18">
@@ -3265,10 +3330,10 @@
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>43952</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>43982</v>
       </c>
       <c r="C19">
@@ -3345,10 +3410,10 @@
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>43983</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>44012</v>
       </c>
       <c r="C20">
@@ -3425,10 +3490,10 @@
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>44013</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>44043</v>
       </c>
       <c r="C21">
@@ -3505,10 +3570,10 @@
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>44044</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>44074</v>
       </c>
       <c r="C22">
@@ -3585,10 +3650,10 @@
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>44075</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>44104</v>
       </c>
       <c r="C23">
@@ -3683,70 +3748,70 @@
       <c r="A1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="1">
         <v>43435</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="1">
         <v>43466</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1" s="4">
         <v>45341</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="1">
         <v>43525</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="1">
         <v>43556</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1" s="1">
         <v>43586</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H1" s="1">
         <v>43617</v>
       </c>
-      <c r="I1" s="2">
+      <c r="I1" s="1">
         <v>43647</v>
       </c>
-      <c r="J1" s="2">
+      <c r="J1" s="1">
         <v>43678</v>
       </c>
-      <c r="K1" s="2">
+      <c r="K1" s="1">
         <v>43709</v>
       </c>
-      <c r="L1" s="2">
+      <c r="L1" s="1">
         <v>43739</v>
       </c>
-      <c r="M1" s="2">
+      <c r="M1" s="1">
         <v>43770</v>
       </c>
-      <c r="N1" s="2">
+      <c r="N1" s="1">
         <v>43800</v>
       </c>
-      <c r="O1" s="2">
+      <c r="O1" s="1">
         <v>43831</v>
       </c>
-      <c r="P1" s="5">
+      <c r="P1" s="4">
         <v>43862</v>
       </c>
-      <c r="Q1" s="2">
+      <c r="Q1" s="1">
         <v>43891</v>
       </c>
-      <c r="R1" s="2">
+      <c r="R1" s="1">
         <v>43922</v>
       </c>
-      <c r="S1" s="2">
+      <c r="S1" s="1">
         <v>43952</v>
       </c>
-      <c r="T1" s="2">
+      <c r="T1" s="1">
         <v>43983</v>
       </c>
-      <c r="U1" s="2">
+      <c r="U1" s="1">
         <v>44013</v>
       </c>
-      <c r="V1" s="2">
+      <c r="V1" s="1">
         <v>44044</v>
       </c>
-      <c r="W1" s="2">
+      <c r="W1" s="1">
         <v>44075</v>
       </c>
     </row>
@@ -3781,7 +3846,7 @@
       <c r="J2">
         <v>17647</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="5">
         <v>16160</v>
       </c>
       <c r="L2">
@@ -3852,7 +3917,7 @@
       <c r="J3">
         <v>14889</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <v>14289</v>
       </c>
       <c r="L3">
@@ -3923,7 +3988,7 @@
       <c r="J4">
         <v>8882</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>9242</v>
       </c>
       <c r="L4">
@@ -3994,7 +4059,7 @@
       <c r="J5">
         <v>7564</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <v>7554</v>
       </c>
       <c r="L5">
@@ -4065,7 +4130,7 @@
       <c r="J6">
         <v>5752</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="5">
         <v>5565</v>
       </c>
       <c r="L6">
@@ -4127,10 +4192,10 @@
       <c r="J7">
         <v>4922</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="5">
         <v>4758</v>
       </c>
-      <c r="M7" s="6"/>
+      <c r="M7" s="5"/>
       <c r="N7">
         <v>4979</v>
       </c>
@@ -4193,7 +4258,7 @@
       <c r="J8">
         <v>6590</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="5">
         <v>6236</v>
       </c>
       <c r="L8">
@@ -4264,7 +4329,7 @@
       <c r="J9">
         <v>5667</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <v>5303</v>
       </c>
       <c r="L9">
@@ -4335,7 +4400,7 @@
       <c r="J10">
         <v>5080</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="5">
         <v>4625</v>
       </c>
       <c r="L10">
@@ -4406,7 +4471,7 @@
       <c r="J11">
         <v>3217</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="5">
         <v>3624</v>
       </c>
       <c r="L11">
@@ -4477,7 +4542,7 @@
       <c r="J12">
         <v>3893</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="5">
         <v>3775</v>
       </c>
       <c r="L12">
@@ -4548,7 +4613,7 @@
       <c r="J13">
         <v>3786</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="5">
         <v>3584</v>
       </c>
       <c r="L13">
@@ -4619,7 +4684,7 @@
       <c r="J14">
         <v>3996</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="5">
         <v>3740</v>
       </c>
       <c r="L14">
@@ -4687,7 +4752,7 @@
       <c r="J15">
         <v>3328</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="5">
         <v>2888</v>
       </c>
       <c r="L15">
@@ -4758,7 +4823,7 @@
       <c r="J16">
         <v>3549</v>
       </c>
-      <c r="K16" s="6">
+      <c r="K16" s="5">
         <v>3778</v>
       </c>
       <c r="L16">
@@ -4829,7 +4894,7 @@
       <c r="J17">
         <v>3737</v>
       </c>
-      <c r="K17" s="6">
+      <c r="K17" s="5">
         <v>3818</v>
       </c>
       <c r="L17">
@@ -4873,7 +4938,7 @@
       <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="M18" s="6"/>
+      <c r="M18" s="5"/>
       <c r="Q18">
         <v>3668</v>
       </c>
@@ -4938,7 +5003,7 @@
       <c r="A20" t="s">
         <v>28</v>
       </c>
-      <c r="M20" s="6"/>
+      <c r="M20" s="5"/>
       <c r="Q20">
         <v>3459</v>
       </c>
@@ -4992,7 +5057,7 @@
       <c r="J21">
         <v>2699</v>
       </c>
-      <c r="K21" s="6">
+      <c r="K21" s="5">
         <v>2563</v>
       </c>
       <c r="L21">
@@ -5071,7 +5136,7 @@
       <c r="J23">
         <v>2839</v>
       </c>
-      <c r="K23" s="6">
+      <c r="K23" s="5">
         <v>2789</v>
       </c>
       <c r="L23">
@@ -5118,13 +5183,13 @@
       <c r="J24">
         <v>2313</v>
       </c>
-      <c r="K24" s="6">
+      <c r="K24" s="5">
         <v>2429</v>
       </c>
       <c r="L24">
         <v>3001</v>
       </c>
-      <c r="M24" s="6"/>
+      <c r="M24" s="5"/>
       <c r="O24">
         <v>2638</v>
       </c>
@@ -5160,7 +5225,7 @@
       <c r="J25">
         <v>2475</v>
       </c>
-      <c r="K25" s="6">
+      <c r="K25" s="5">
         <v>2430</v>
       </c>
       <c r="L25">
@@ -5206,10 +5271,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF1B4C0C-9C23-A741-8FA6-B4F49FBA7F21}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5227,1109 +5292,1245 @@
     <col min="13" max="13" width="24" customWidth="1"/>
     <col min="14" max="14" width="18.1640625" customWidth="1"/>
     <col min="15" max="15" width="24.6640625" customWidth="1"/>
+    <col min="16" max="16" width="62.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>47</v>
       </c>
       <c r="L1" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>44</v>
       </c>
       <c r="O1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
+      <c r="P1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
         <v>44896</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>44926</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>217884</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <f>ROUND(C2/(B2-A2), 0)</f>
         <v>7263</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>1</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>95853</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <f>(C2-F2)</f>
         <v>122031</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <f>ROUND(G2/(B2-A2), 0)</f>
         <v>4068</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>638</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="5">
         <v>0</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="5">
         <v>1907</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="2">
         <v>243351</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="2">
         <v>293813</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="5">
         <f>ROUND(M2/(B2-A2), 0)</f>
         <v>9794</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
+      <c r="O2" s="2">
+        <v>1050</v>
+      </c>
+      <c r="P2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
         <v>44927</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>44957</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>215981</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <f t="shared" ref="D3:D23" si="0">ROUND(C3/(B3-A3), 0)</f>
         <v>7199</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>94208</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <f t="shared" ref="G3:G23" si="1">(C3-F3)</f>
         <v>121773</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <f t="shared" ref="H3:H23" si="2">ROUND(G3/(B3-A3), 0)</f>
         <v>4059</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <v>546</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <v>0</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <v>1940</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="2">
         <v>208912</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="2">
         <v>254979</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="5">
         <f t="shared" ref="N3:N22" si="3">ROUND(M3/(B3-A3), 0)</f>
         <v>8499</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
+      <c r="O3" s="2">
+        <v>1070</v>
+      </c>
+      <c r="P3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
         <v>44958</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>44985</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>190210</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <f t="shared" si="0"/>
         <v>7045</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>1</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>83160</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <f t="shared" si="1"/>
         <v>107050</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <f t="shared" si="2"/>
         <v>3965</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>544</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>0</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>1944</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="2">
         <v>176485</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="2">
         <v>332270</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="5">
         <f t="shared" si="3"/>
         <v>12306</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+      <c r="O4" s="2">
+        <v>1060</v>
+      </c>
+      <c r="P4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
         <v>44986</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>45016</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>195874</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <f t="shared" si="0"/>
         <v>6529</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>1</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>85512</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <f t="shared" si="1"/>
         <v>110362</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <f t="shared" si="2"/>
         <v>3679</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>596</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>0</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <v>2002</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="2">
         <v>219329</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="2">
         <v>378028</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="5">
         <f t="shared" si="3"/>
         <v>12601</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
+      <c r="O5" s="2">
+        <v>1083</v>
+      </c>
+      <c r="P5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
         <v>45017</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>45046</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>153940</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <f t="shared" si="0"/>
         <v>5308</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>1</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>68033</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <f t="shared" si="1"/>
         <v>85907</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <f t="shared" si="2"/>
         <v>2962</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>582</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <v>0</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="5">
         <v>2070</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="2">
         <v>233615</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="2">
         <v>302718</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="5">
         <f t="shared" si="3"/>
         <v>10439</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+      <c r="O6" s="2">
+        <v>1117</v>
+      </c>
+      <c r="P6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
         <v>45047</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>45077</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>147842</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <f t="shared" si="0"/>
         <v>4928</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>1</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>64887</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <f t="shared" si="1"/>
         <v>82955</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <f t="shared" si="2"/>
         <v>2765</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>555</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <v>0</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="5">
         <v>2102</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="2">
         <v>203828</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="2">
         <v>285696</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="5">
         <f t="shared" si="3"/>
         <v>9523</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
+      <c r="O7" s="2">
+        <v>1127</v>
+      </c>
+      <c r="P7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
         <v>45078</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>45107</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>140533</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <f t="shared" si="0"/>
         <v>4846</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>1</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>62371</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <f t="shared" si="1"/>
         <v>78162</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <f t="shared" si="2"/>
         <v>2695</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <v>498</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <v>0</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="5">
         <v>2097</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="2">
         <v>153980</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="2">
         <v>229344</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="5">
         <f t="shared" si="3"/>
         <v>7908</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
+      <c r="O8" s="2">
+        <v>1117</v>
+      </c>
+      <c r="P8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
         <v>45108</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>45138</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>139682</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <f t="shared" si="0"/>
         <v>4656</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>1</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>61487</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <f t="shared" si="1"/>
         <v>78195</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <f t="shared" si="2"/>
         <v>2607</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>466</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>0</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <v>2118</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="2">
         <v>152139</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="2">
         <v>212314</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="5">
         <f t="shared" si="3"/>
         <v>7077</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
+      <c r="O9" s="2">
+        <v>1124</v>
+      </c>
+      <c r="P9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
         <v>45139</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>45169</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>135465</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <f t="shared" si="0"/>
         <v>4516</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>1</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>58995</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <f t="shared" si="1"/>
         <v>76470</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <f t="shared" si="2"/>
         <v>2549</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <v>439</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="5">
         <v>0</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="5">
         <v>2129</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="2">
         <v>155231</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="2">
         <v>216396</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="5">
         <f t="shared" si="3"/>
         <v>7213</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
+      <c r="O10" s="2">
+        <v>1135</v>
+      </c>
+      <c r="P10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
         <v>45170</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>45199</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>123453</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <f t="shared" si="0"/>
         <v>4257</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>1</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>53484</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <f t="shared" si="1"/>
         <v>69969</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <f t="shared" si="2"/>
         <v>2413</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <v>413</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="5">
         <v>0</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="5">
         <v>2117</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="2">
         <v>177374</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="2">
         <v>224741</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="5">
         <f t="shared" si="3"/>
         <v>7750</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
+      <c r="O11" s="2">
+        <v>1132</v>
+      </c>
+      <c r="P11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
         <v>45200</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>45230</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>134191</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <f t="shared" si="0"/>
         <v>4473</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>1</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>65817</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <f t="shared" si="1"/>
         <v>68374</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <f t="shared" si="2"/>
         <v>2279</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="2">
         <v>329</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="5">
         <v>0</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="5">
         <v>2110</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L12" s="2">
         <v>165054</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M12" s="2">
         <v>224727</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="5">
         <f t="shared" si="3"/>
         <v>7491</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
+      <c r="O12" s="2">
+        <v>1134</v>
+      </c>
+      <c r="P12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
         <v>45231</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>45260</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>128104</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <f t="shared" si="0"/>
         <v>4417</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>1</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>63367</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <f t="shared" si="1"/>
         <v>64737</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <f t="shared" si="2"/>
         <v>2232</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="2">
         <v>300</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="5">
         <v>0</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="5">
         <v>2165</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="2">
         <v>172308</v>
       </c>
-      <c r="M13" s="1">
+      <c r="M13" s="2">
         <v>228129</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="5">
         <f t="shared" si="3"/>
         <v>7867</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="7">
+      <c r="O13" s="2">
+        <v>1149</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
         <v>45261</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>45291</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>111414</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <f t="shared" si="0"/>
         <v>3714</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>1</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>55028</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="5">
         <f t="shared" si="1"/>
         <v>56386</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="5">
         <f t="shared" si="2"/>
         <v>1880</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="2">
         <v>253</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="5">
         <v>0</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="5">
         <v>2208</v>
       </c>
-      <c r="L14" s="1">
+      <c r="L14" s="2">
         <v>156972</v>
       </c>
-      <c r="M14" s="1">
+      <c r="M14" s="2">
         <v>216645</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="5">
         <f t="shared" si="3"/>
         <v>7222</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="7">
+      <c r="O14" s="2">
+        <v>1197</v>
+      </c>
+      <c r="P14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
         <v>45292</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>45322</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>122524</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <f t="shared" si="0"/>
         <v>4084</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>1</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <v>59813</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <f t="shared" si="1"/>
         <v>62711</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <f t="shared" si="2"/>
         <v>2090</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="2">
         <v>228</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="5">
         <v>0</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="5">
         <v>2200</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L15" s="2">
         <v>141607</v>
       </c>
-      <c r="M15" s="1">
+      <c r="M15" s="2">
         <v>195823</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="5">
         <f t="shared" si="3"/>
         <v>6527</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="7">
+      <c r="O15" s="2">
+        <v>1184</v>
+      </c>
+      <c r="P15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
         <v>45323</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>45350</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>112812</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <f t="shared" si="0"/>
         <v>4178</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>1</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <v>55863</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="5">
         <f t="shared" si="1"/>
         <v>56949</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="5">
         <f t="shared" si="2"/>
         <v>2109</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="2">
         <v>207</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J16" s="5">
         <v>0</v>
       </c>
-      <c r="K16" s="6">
+      <c r="K16" s="5">
         <v>2172</v>
       </c>
-      <c r="L16" s="1">
+      <c r="L16" s="2">
         <v>161967</v>
       </c>
-      <c r="M16" s="1">
+      <c r="M16" s="2">
         <v>206784</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="5">
         <f t="shared" si="3"/>
         <v>7659</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="7">
+      <c r="O16" s="2">
+        <v>1176</v>
+      </c>
+      <c r="P16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
         <v>45352</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>45382</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>118558</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <f t="shared" si="0"/>
         <v>3952</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>1</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="2">
         <v>58522</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <f t="shared" si="1"/>
         <v>60036</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <f t="shared" si="2"/>
         <v>2001</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="2">
         <v>165</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J17" s="5">
         <v>0</v>
       </c>
-      <c r="K17" s="6">
+      <c r="K17" s="5">
         <v>2246</v>
       </c>
-      <c r="L17" s="1">
+      <c r="L17" s="2">
         <v>400808</v>
       </c>
-      <c r="M17" s="1">
+      <c r="M17" s="2">
         <v>299206</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="5">
         <f t="shared" si="3"/>
         <v>9974</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
+      <c r="O17" s="2">
+        <v>1186</v>
+      </c>
+      <c r="P17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
         <v>45383</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <v>45412</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>110521</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <f t="shared" si="0"/>
         <v>3811</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>1</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="2">
         <v>55289</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="5">
         <f t="shared" si="1"/>
         <v>55232</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="5">
         <f t="shared" si="2"/>
         <v>1905</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="2">
         <v>139</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J18" s="5">
         <v>0</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="5">
         <v>2256</v>
       </c>
-      <c r="L18" s="1">
+      <c r="L18" s="2">
         <v>858680</v>
       </c>
-      <c r="M18" s="1">
+      <c r="M18" s="2">
         <v>633184</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="5">
         <f t="shared" si="3"/>
         <v>21834</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="7">
+      <c r="O18" s="2">
+        <v>1186</v>
+      </c>
+      <c r="P18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
         <v>45413</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>45443</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>106668</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <f t="shared" si="0"/>
         <v>3556</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>1</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <v>52602</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="5">
         <f t="shared" si="1"/>
         <v>54066</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="5">
         <f t="shared" si="2"/>
         <v>1802</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="2">
         <v>136</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="5">
         <v>0</v>
       </c>
-      <c r="K19" s="6">
+      <c r="K19" s="5">
         <v>2298</v>
       </c>
-      <c r="L19" s="1">
+      <c r="L19" s="2">
         <v>522539</v>
       </c>
-      <c r="M19" s="1">
+      <c r="M19" s="2">
         <v>653516</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="5">
         <f t="shared" si="3"/>
         <v>21784</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="7">
+      <c r="O19" s="2">
+        <v>1194</v>
+      </c>
+      <c r="P19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
         <v>45444</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <v>45473</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>86358</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <f t="shared" si="0"/>
         <v>2978</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>1</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>41297</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="5">
         <f t="shared" si="1"/>
         <v>45061</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="5">
         <f t="shared" si="2"/>
         <v>1554</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="2">
         <v>126</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J20" s="5">
         <v>0</v>
       </c>
-      <c r="K20" s="6">
+      <c r="K20" s="5">
         <v>2381</v>
       </c>
-      <c r="L20" s="1">
+      <c r="L20" s="2">
         <v>492759</v>
       </c>
-      <c r="M20" s="1">
+      <c r="M20" s="2">
         <v>670362</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="5">
         <f t="shared" si="3"/>
         <v>23116</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="7">
+      <c r="O20" s="2">
+        <v>1199</v>
+      </c>
+      <c r="P20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
         <v>45474</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <v>45504</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>86444</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <f t="shared" si="0"/>
         <v>2881</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>1</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <v>41323</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="5">
         <f t="shared" si="1"/>
         <v>45121</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="5">
         <f t="shared" si="2"/>
         <v>1504</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="2">
         <v>99</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J21" s="5">
         <v>0</v>
       </c>
-      <c r="K21" s="6">
+      <c r="K21" s="5">
         <v>2400</v>
       </c>
-      <c r="L21" s="1">
+      <c r="L21" s="2">
         <v>700025</v>
       </c>
-      <c r="M21" s="1">
+      <c r="M21" s="2">
         <v>977051</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="5">
         <f t="shared" si="3"/>
         <v>32568</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="7">
+      <c r="O21" s="2">
+        <v>1180</v>
+      </c>
+      <c r="P21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
         <v>45505</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <v>45535</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>79712</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <f t="shared" si="0"/>
         <v>2657</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>1</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>37031</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="5">
         <f t="shared" si="1"/>
         <v>42681</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="5">
         <f t="shared" si="2"/>
         <v>1423</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="2">
         <v>84</v>
       </c>
-      <c r="J22" s="6">
+      <c r="J22" s="5">
         <v>0</v>
       </c>
-      <c r="K22" s="6">
+      <c r="K22" s="5">
         <v>2421</v>
       </c>
-      <c r="L22" s="1">
+      <c r="L22" s="2">
         <v>495257</v>
       </c>
-      <c r="M22" s="1">
+      <c r="M22" s="2">
         <v>861132</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="5">
         <f t="shared" si="3"/>
         <v>28704</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="7">
+      <c r="O22" s="2">
+        <v>1199</v>
+      </c>
+      <c r="P22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
         <v>45536</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="6">
         <v>45565</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>73564</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <f t="shared" si="0"/>
         <v>2537</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>1</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>36310</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="5">
         <f t="shared" si="1"/>
         <v>37254</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="5">
         <f t="shared" si="2"/>
         <v>1285</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="2">
         <v>52</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="2">
         <v>0</v>
       </c>
-      <c r="K23" s="3">
+      <c r="K23" s="2">
         <v>2359</v>
       </c>
-      <c r="L23" s="1">
+      <c r="L23" s="2">
         <v>371754</v>
       </c>
-      <c r="M23" s="1">
+      <c r="M23" s="2">
         <v>1291032</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="5">
         <f>ROUND(M23/(B23-A23), 0)</f>
         <v>44518</v>
+      </c>
+      <c r="O23" s="2">
+        <v>1229</v>
+      </c>
+      <c r="P23" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6357,84 +6558,84 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4">
+      <c r="C1" s="3">
         <v>0</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="3">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="3">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="3">
         <v>0.125</v>
       </c>
-      <c r="G1" s="4">
+      <c r="G1" s="3">
         <v>0.16666666666666666</v>
       </c>
-      <c r="H1" s="4">
+      <c r="H1" s="3">
         <v>0.20833333333333334</v>
       </c>
-      <c r="I1" s="4">
+      <c r="I1" s="3">
         <v>0.25</v>
       </c>
-      <c r="J1" s="4">
+      <c r="J1" s="3">
         <v>0.29166666666666669</v>
       </c>
-      <c r="K1" s="4">
+      <c r="K1" s="3">
         <v>0.33333333333333331</v>
       </c>
-      <c r="L1" s="4">
+      <c r="L1" s="3">
         <v>0.375</v>
       </c>
-      <c r="M1" s="4">
+      <c r="M1" s="3">
         <v>0.41666666666666669</v>
       </c>
-      <c r="N1" s="4">
+      <c r="N1" s="3">
         <v>0.45833333333333331</v>
       </c>
-      <c r="O1" s="4">
+      <c r="O1" s="3">
         <v>0.5</v>
       </c>
-      <c r="P1" s="4">
+      <c r="P1" s="3">
         <v>0.54166666666666663</v>
       </c>
-      <c r="Q1" s="4">
+      <c r="Q1" s="3">
         <v>0.58333333333333337</v>
       </c>
-      <c r="R1" s="4">
+      <c r="R1" s="3">
         <v>0.625</v>
       </c>
-      <c r="S1" s="4">
+      <c r="S1" s="3">
         <v>0.66666666666666663</v>
       </c>
-      <c r="T1" s="4">
+      <c r="T1" s="3">
         <v>0.70833333333333337</v>
       </c>
-      <c r="U1" s="4">
+      <c r="U1" s="3">
         <v>0.75</v>
       </c>
-      <c r="V1" s="4">
+      <c r="V1" s="3">
         <v>0.79166666666666663</v>
       </c>
-      <c r="W1" s="4">
+      <c r="W1" s="3">
         <v>0.83333333333333337</v>
       </c>
-      <c r="X1" s="4">
+      <c r="X1" s="3">
         <v>0.875</v>
       </c>
-      <c r="Y1" s="4">
+      <c r="Y1" s="3">
         <v>0.91666666666666663</v>
       </c>
-      <c r="Z1" s="4">
+      <c r="Z1" s="3">
         <v>0.95833333333333337</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>44896</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>44926</v>
       </c>
       <c r="C2">
@@ -6511,10 +6712,10 @@
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>44927</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>44957</v>
       </c>
       <c r="C3">
@@ -6591,10 +6792,10 @@
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>44958</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>44985</v>
       </c>
       <c r="C4">
@@ -6671,10 +6872,10 @@
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>44986</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>45016</v>
       </c>
       <c r="C5">
@@ -6751,10 +6952,10 @@
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>45017</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>45046</v>
       </c>
       <c r="C6">
@@ -6831,10 +7032,10 @@
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>45047</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>45077</v>
       </c>
       <c r="C7">
@@ -6911,10 +7112,10 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>45078</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>45107</v>
       </c>
       <c r="C8">
@@ -6991,10 +7192,10 @@
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>45108</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>45138</v>
       </c>
       <c r="C9">
@@ -7071,10 +7272,10 @@
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>45139</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>45169</v>
       </c>
       <c r="C10">
@@ -7151,10 +7352,10 @@
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>45170</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>45199</v>
       </c>
       <c r="C11">
@@ -7231,10 +7432,10 @@
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>45200</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>45230</v>
       </c>
       <c r="C12">
@@ -7311,10 +7512,10 @@
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>45231</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>45260</v>
       </c>
       <c r="C13">
@@ -7391,10 +7592,10 @@
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>45261</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>45291</v>
       </c>
       <c r="C14">
@@ -7471,10 +7672,10 @@
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>45292</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>45322</v>
       </c>
       <c r="C15">
@@ -7551,10 +7752,10 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>45323</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>45350</v>
       </c>
       <c r="C16">
@@ -7631,10 +7832,10 @@
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>45352</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>45382</v>
       </c>
       <c r="C17">
@@ -7711,10 +7912,10 @@
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>45383</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>45412</v>
       </c>
       <c r="C18">
@@ -7791,10 +7992,10 @@
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>45413</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>45443</v>
       </c>
       <c r="C19">
@@ -7871,10 +8072,10 @@
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>45444</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>45473</v>
       </c>
       <c r="C20">
@@ -7951,10 +8152,10 @@
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>45474</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>45504</v>
       </c>
       <c r="C21">
@@ -8031,10 +8232,10 @@
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>45505</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>45535</v>
       </c>
       <c r="C22">
@@ -8111,10 +8312,10 @@
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>45536</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>45565</v>
       </c>
       <c r="C23">
@@ -8199,7 +8400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A778379-CFC1-4B42-A0D1-2736402F63AF}">
   <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
@@ -8209,70 +8410,70 @@
       <c r="A1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="1">
         <v>44896</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="1">
         <v>44927</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="1">
         <v>44958</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="1">
         <v>44986</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="1">
         <v>45017</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1" s="1">
         <v>45047</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H1" s="1">
         <v>45078</v>
       </c>
-      <c r="I1" s="2">
+      <c r="I1" s="1">
         <v>45108</v>
       </c>
-      <c r="J1" s="2">
+      <c r="J1" s="1">
         <v>45139</v>
       </c>
-      <c r="K1" s="2">
+      <c r="K1" s="1">
         <v>45170</v>
       </c>
-      <c r="L1" s="2">
+      <c r="L1" s="1">
         <v>45200</v>
       </c>
-      <c r="M1" s="2">
+      <c r="M1" s="1">
         <v>45231</v>
       </c>
-      <c r="N1" s="2">
+      <c r="N1" s="1">
         <v>45261</v>
       </c>
-      <c r="O1" s="2">
+      <c r="O1" s="1">
         <v>45292</v>
       </c>
-      <c r="P1" s="2">
+      <c r="P1" s="1">
         <v>45323</v>
       </c>
-      <c r="Q1" s="2">
+      <c r="Q1" s="1">
         <v>45352</v>
       </c>
-      <c r="R1" s="2">
+      <c r="R1" s="1">
         <v>45383</v>
       </c>
-      <c r="S1" s="2">
+      <c r="S1" s="1">
         <v>45413</v>
       </c>
-      <c r="T1" s="2">
+      <c r="T1" s="1">
         <v>45444</v>
       </c>
-      <c r="U1" s="2">
+      <c r="U1" s="1">
         <v>45474</v>
       </c>
-      <c r="V1" s="2">
+      <c r="V1" s="1">
         <v>45505</v>
       </c>
-      <c r="W1" s="2">
+      <c r="W1" s="1">
         <v>45536</v>
       </c>
     </row>
@@ -9450,14 +9651,14 @@
       <c r="A23" t="s">
         <v>30</v>
       </c>
-      <c r="K23" s="6"/>
+      <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>31</v>
       </c>
-      <c r="K24" s="6"/>
-      <c r="M24" s="6"/>
+      <c r="K24" s="5"/>
+      <c r="M24" s="5"/>
       <c r="V24">
         <v>692</v>
       </c>
@@ -9466,7 +9667,7 @@
       <c r="A25" t="s">
         <v>32</v>
       </c>
-      <c r="K25" s="6"/>
+      <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" t="s">

</xml_diff>

<commit_message>
push graphs to github
</commit_message>
<xml_diff>
--- a/excel_files/Stack Overflow Data Collection.xlsx
+++ b/excel_files/Stack Overflow Data Collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coltonpalfrey/Desktop/PASCL RA/Stack-Overflow-Data-Analysis/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D76984-CD4A-2E44-A33C-51C7DF233BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB49F51-359E-C741-AC11-D32D3CF9D47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="2560" windowWidth="33600" windowHeight="18760" activeTab="1" xr2:uid="{1E05B25D-E817-2248-B7C5-0489F78289AB}"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="4" xr2:uid="{1E05B25D-E817-2248-B7C5-0489F78289AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Pre LLM monthly data" sheetId="1" r:id="rId1"/>
@@ -21823,7 +21823,7 @@
   <dimension ref="A1:W25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B23"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23117,7 +23117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{325E82BB-BF2D-5841-A148-1F4624B2FC06}">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -23157,7 +23157,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43435</v>
       </c>
@@ -23209,7 +23209,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43435</v>
       </c>
@@ -23235,7 +23235,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43435</v>
       </c>
@@ -23339,7 +23339,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43466</v>
       </c>
@@ -23391,7 +23391,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43466</v>
       </c>
@@ -23417,7 +23417,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43497</v>
       </c>
@@ -23495,7 +23495,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43497</v>
       </c>
@@ -23547,7 +23547,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43525</v>
       </c>
@@ -23573,7 +23573,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43525</v>
       </c>
@@ -23599,7 +23599,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43525</v>
       </c>
@@ -23651,7 +23651,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43525</v>
       </c>
@@ -23677,7 +23677,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43556</v>
       </c>
@@ -23703,7 +23703,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43556</v>
       </c>
@@ -23781,7 +23781,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43556</v>
       </c>
@@ -23807,7 +23807,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43586</v>
       </c>
@@ -23885,7 +23885,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43586</v>
       </c>
@@ -23911,7 +23911,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43586</v>
       </c>
@@ -23937,7 +23937,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43617</v>
       </c>
@@ -23963,7 +23963,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43617</v>
       </c>
@@ -23989,7 +23989,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43617</v>
       </c>
@@ -24015,7 +24015,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43617</v>
       </c>
@@ -24041,7 +24041,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43617</v>
       </c>
@@ -24067,7 +24067,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43647</v>
       </c>
@@ -24119,7 +24119,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>43647</v>
       </c>
@@ -24145,7 +24145,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>43647</v>
       </c>
@@ -24223,7 +24223,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>43678</v>
       </c>
@@ -24249,7 +24249,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43678</v>
       </c>
@@ -24275,7 +24275,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43678</v>
       </c>
@@ -24301,7 +24301,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>43678</v>
       </c>
@@ -24353,7 +24353,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>43709</v>
       </c>
@@ -24379,7 +24379,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>43709</v>
       </c>
@@ -24405,7 +24405,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>43709</v>
       </c>
@@ -24431,7 +24431,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>43709</v>
       </c>
@@ -24457,7 +24457,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>43739</v>
       </c>
@@ -24509,7 +24509,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>43739</v>
       </c>
@@ -24613,7 +24613,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>43770</v>
       </c>
@@ -24639,7 +24639,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>43770</v>
       </c>
@@ -24769,7 +24769,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>43800</v>
       </c>
@@ -24795,7 +24795,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>43800</v>
       </c>
@@ -24873,7 +24873,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>43831</v>
       </c>
@@ -25029,7 +25029,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>43862</v>
       </c>
@@ -25185,7 +25185,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>43891</v>
       </c>
@@ -25237,7 +25237,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>43922</v>
       </c>
@@ -25289,7 +25289,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>43922</v>
       </c>
@@ -25341,7 +25341,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>43922</v>
       </c>
@@ -25367,7 +25367,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>43952</v>
       </c>
@@ -25471,7 +25471,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>43952</v>
       </c>
@@ -25523,7 +25523,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>43983</v>
       </c>
@@ -25549,7 +25549,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>43983</v>
       </c>
@@ -29416,8 +29416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF1B4C0C-9C23-A741-8FA6-B4F49FBA7F21}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B23"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30928,7 +30928,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="388" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="119" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>44958</v>
       </c>
@@ -30988,7 +30988,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="221" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>44958</v>
       </c>
@@ -31068,7 +31068,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="289" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>44986</v>
       </c>
@@ -31128,7 +31128,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="388" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>45017</v>
       </c>
@@ -31188,7 +31188,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>45017</v>
       </c>
@@ -31208,7 +31208,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="221" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>45017</v>
       </c>
@@ -31288,7 +31288,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="289" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>45047</v>
       </c>
@@ -31388,7 +31388,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="356" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>45078</v>
       </c>
@@ -31808,7 +31808,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="404" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
         <v>45200</v>
       </c>
@@ -31888,7 +31888,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="323" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
         <v>45231</v>
       </c>
@@ -31968,7 +31968,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" ht="306" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
         <v>45261</v>
       </c>
@@ -32088,7 +32088,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" ht="289" x14ac:dyDescent="0.2">
       <c r="A70" s="6">
         <v>45292</v>
       </c>
@@ -32108,7 +32108,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" ht="306" x14ac:dyDescent="0.2">
       <c r="A71" s="6">
         <v>45292</v>
       </c>
@@ -32168,7 +32168,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" ht="306" x14ac:dyDescent="0.2">
       <c r="A74" s="6">
         <v>45323</v>
       </c>
@@ -32228,7 +32228,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" ht="272" x14ac:dyDescent="0.2">
       <c r="A77" s="6">
         <v>45352</v>
       </c>
@@ -32288,7 +32288,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" ht="221" x14ac:dyDescent="0.2">
       <c r="A80" s="6">
         <v>45352</v>
       </c>
@@ -32648,7 +32648,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" ht="170" x14ac:dyDescent="0.2">
       <c r="A98" s="6">
         <v>45474</v>
       </c>

</xml_diff>